<commit_message>
Filled in more of grading guide.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Current\DSAII\OrBITS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\twb1193\IGMProfile\Desktop\GitHub\orbits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Gravity requires all of these</t>
+  </si>
+  <si>
+    <t>Textures</t>
   </si>
 </sst>
 </file>
@@ -808,6 +811,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,24 +865,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -847,14 +874,23 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -863,70 +899,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1212,7 +1215,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,58 +1799,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="70" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
-        <v>35.714285714285715</v>
+        <v>60.714285714285708</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="71" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1863,25 +1866,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1890,12 +1893,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1908,24 +1911,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1938,12 +1941,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -1954,12 +1957,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1972,12 +1975,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -1986,12 +1989,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2004,24 +2007,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2030,12 +2033,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2044,12 +2047,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2058,12 +2061,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2076,24 +2079,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2102,12 +2105,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2116,309 +2119,311 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="12">
+        <v>20</v>
+      </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
       </c>
       <c r="F23" s="9">
         <f>SUM(F20:F22)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2427,12 +2432,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2441,12 +2446,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2459,25 +2464,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2486,12 +2491,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2500,26 +2505,28 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
-      <c r="F52" s="12"/>
+      <c r="F52" s="12">
+        <v>5</v>
+      </c>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2528,26 +2535,28 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
-      <c r="F54" s="12"/>
+      <c r="F54" s="12">
+        <v>10</v>
+      </c>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2556,12 +2565,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2572,12 +2581,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2586,12 +2595,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2600,12 +2609,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2614,12 +2623,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2628,12 +2637,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2644,12 +2653,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2658,12 +2667,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2672,12 +2681,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2686,12 +2695,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2700,12 +2709,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2714,12 +2723,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2728,51 +2737,53 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="29"/>
-      <c r="G68" s="22"/>
+      <c r="G68" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
       </c>
       <c r="F69" s="32">
         <f>SUM(F50:F68)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
       </c>
       <c r="F70" s="31">
         <f>MAX(0,SUM(F7,F13,F18,F23,F48,F69))</f>
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
@@ -3352,35 +3363,43 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="A64:D64"/>
@@ -3397,43 +3416,35 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made planet trails more efficient.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\twb1193\IGMProfile\Desktop\GitHub\orbits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Current\DSAII\ORBITZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -811,6 +811,93 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -843,93 +930,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,58 +1799,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="41" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="42" t="s">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73">
         <f>((F70/E70)*100)</f>
         <v>60.714285714285708</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1866,25 +1866,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1893,12 +1893,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1911,24 +1911,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1941,12 +1941,12 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
@@ -1957,12 +1957,12 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1975,12 +1975,12 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
@@ -1989,12 +1989,12 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
@@ -2007,24 +2007,24 @@
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
@@ -2033,12 +2033,12 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
@@ -2047,12 +2047,12 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2061,12 +2061,12 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
@@ -2079,24 +2079,24 @@
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
@@ -2105,12 +2105,12 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
@@ -2119,12 +2119,12 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2135,12 +2135,12 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
@@ -2153,277 +2153,277 @@
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2432,12 +2432,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2446,12 +2446,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="69"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="70"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2464,25 +2464,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="64"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="51"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2491,12 +2491,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="51"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2505,12 +2505,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="51"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2521,12 +2521,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+      <c r="A53" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="51"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2535,12 +2535,12 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="51"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
@@ -2551,12 +2551,12 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="51"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2565,12 +2565,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="51"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2581,12 +2581,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="51"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2595,12 +2595,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="51"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2609,12 +2609,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="51"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2623,12 +2623,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="51"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2637,12 +2637,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="51"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2653,12 +2653,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="51"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2667,12 +2667,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="51"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2681,12 +2681,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="51"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2695,12 +2695,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="51"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2709,12 +2709,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="51"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2723,12 +2723,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="51"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2737,12 +2737,12 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="51"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
@@ -2753,12 +2753,12 @@
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="52" t="s">
+      <c r="A69" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="54"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="46"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
@@ -2771,12 +2771,12 @@
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="73"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="43"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
@@ -3363,6 +3363,72 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E34:H34"/>
@@ -3379,72 +3445,6 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added container for octree. Added collision for all asteroids. Added oscillating skewing to the bezier surface.
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Current\DSAII\ORBITZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\banner.main.ad.rit.edu\students\twb1193\IGMProfile\Desktop\GitHub\orbits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Textures</t>
+  </si>
+  <si>
+    <t>Collision preserves/transfers momentum</t>
+  </si>
+  <si>
+    <t>Visual evident in collision of bodies</t>
+  </si>
+  <si>
+    <t>Sphere-sphere</t>
   </si>
 </sst>
 </file>
@@ -811,6 +820,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,24 +874,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -850,14 +883,23 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -866,70 +908,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1215,7 +1224,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,58 +1808,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="70" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="71" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
-        <v>60.714285714285708</v>
+        <v>96.428571428571431</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="71" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1866,25 +1875,25 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="6">
         <v>10</v>
       </c>
@@ -1893,12 +1902,12 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
       <c r="E7" s="8">
         <f>SUM(E6:E6)</f>
         <v>10</v>
@@ -1911,24 +1920,24 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="12">
         <v>10</v>
       </c>
@@ -1941,28 +1950,30 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
       <c r="F10" s="12">
         <v>10</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="12">
         <v>10</v>
       </c>
@@ -1975,84 +1986,94 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="12">
         <v>10</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="F12" s="12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="8">
         <f>SUM(E9:E12)</f>
         <v>40</v>
       </c>
       <c r="F13" s="9">
         <f>SUM(F9:F12)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>10</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="F15" s="12">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <v>10</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="12">
+        <v>10</v>
+      </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="12">
         <v>40</v>
       </c>
@@ -2061,70 +2082,74 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="8">
         <f>SUM(E15:E17)</f>
         <v>60</v>
       </c>
       <c r="F18" s="9">
         <f>SUM(F15:F17)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="12">
         <v>5</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="12">
+        <v>5</v>
+      </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="12">
         <v>5</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="12">
+        <v>5</v>
+      </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="12">
         <v>20</v>
       </c>
@@ -2135,295 +2160,295 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="8">
         <f>SUM(E20:E22)</f>
         <v>30</v>
       </c>
       <c r="F23" s="9">
         <f>SUM(F20:F22)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="29.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="37"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:10" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="37"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="37"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="37"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="21"/>
     </row>
     <row r="46" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="37"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25"/>
       <c r="G46" s="26"/>
@@ -2432,12 +2457,12 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="12"/>
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
@@ -2446,12 +2471,12 @@
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="14">
         <f>SUM(E26:E47)</f>
         <v>0</v>
@@ -2464,25 +2489,25 @@
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="54"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="56"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="64"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="37"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="12">
         <v>5</v>
       </c>
@@ -2491,12 +2516,12 @@
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="12">
         <v>5</v>
       </c>
@@ -2505,12 +2530,12 @@
       <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="12">
         <v>5</v>
       </c>
@@ -2521,12 +2546,12 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="37"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
       <c r="E53" s="12">
         <v>10</v>
       </c>
@@ -2535,28 +2560,28 @@
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="37"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="12">
         <v>50</v>
       </c>
       <c r="F54" s="12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="12">
         <v>10</v>
       </c>
@@ -2565,12 +2590,12 @@
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="37"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="12">
         <v>10</v>
       </c>
@@ -2581,12 +2606,12 @@
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="37"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="E57" s="12">
         <v>20</v>
       </c>
@@ -2595,12 +2620,12 @@
       <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="37"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="12">
         <v>20</v>
       </c>
@@ -2609,12 +2634,12 @@
       <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="37"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="51"/>
       <c r="E59" s="12">
         <v>20</v>
       </c>
@@ -2623,12 +2648,12 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="37"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="51"/>
       <c r="E60" s="12">
         <v>30</v>
       </c>
@@ -2637,12 +2662,12 @@
       <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="37"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
       <c r="E61" s="12">
         <v>10</v>
       </c>
@@ -2653,12 +2678,12 @@
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="51"/>
       <c r="E62" s="12">
         <v>20</v>
       </c>
@@ -2667,12 +2692,12 @@
       <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="37"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="51"/>
       <c r="E63" s="12">
         <v>30</v>
       </c>
@@ -2681,12 +2706,12 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="51"/>
       <c r="E64" s="12">
         <v>20</v>
       </c>
@@ -2695,12 +2720,12 @@
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="37"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="51"/>
       <c r="E65" s="12">
         <v>20</v>
       </c>
@@ -2709,12 +2734,12 @@
       <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="37"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="51"/>
       <c r="E66" s="12">
         <v>20</v>
       </c>
@@ -2723,12 +2748,12 @@
       <c r="H66" s="13"/>
     </row>
     <row r="67" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="37"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="51"/>
       <c r="E67" s="12">
         <v>20</v>
       </c>
@@ -2737,12 +2762,12 @@
       <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="37"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="51"/>
       <c r="E68" s="24" t="s">
         <v>25</v>
       </c>
@@ -2753,37 +2778,37 @@
       <c r="H68" s="22"/>
     </row>
     <row r="69" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="33">
         <f>SUM(E50:E67)</f>
         <v>325</v>
       </c>
       <c r="F69" s="32">
         <f>SUM(F50:F68)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="73"/>
       <c r="E70" s="30">
         <f>SUM(E7,E13,E18,E23)</f>
         <v>140</v>
       </c>
       <c r="F70" s="31">
         <f>MAX(0,SUM(F7,F13,F18,F23,F48,F69))</f>
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
@@ -3363,35 +3388,43 @@
     <row r="153" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="A64:D64"/>
@@ -3408,43 +3441,35 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Octree and finished up project (menus and small requirements, etc).
</commit_message>
<xml_diff>
--- a/DSA2 Final Grading Guide.xlsx
+++ b/DSA2 Final Grading Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>IGME 309 Final Project Fall 2013 Grading Guide</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Implement a custom GUI system.</t>
   </si>
   <si>
-    <t>Tommey Bentley</t>
-  </si>
-  <si>
     <t>Jacob Burdecki</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>Gravity requires all of these</t>
   </si>
   <si>
-    <t>Textures</t>
-  </si>
-  <si>
     <t>Collision preserves/transfers momentum</t>
   </si>
   <si>
@@ -274,6 +268,42 @@
   </si>
   <si>
     <t>Sphere-sphere</t>
+  </si>
+  <si>
+    <t>Bezier surface in main menu is scaled.</t>
+  </si>
+  <si>
+    <t>Bezier surface is continuously sheared in a sinusoidal pattern.</t>
+  </si>
+  <si>
+    <t>Octree is implemented(class Octree) and used(Source.cpp line ….)</t>
+  </si>
+  <si>
+    <t>Collision detection prevents tunneling (also it is visually evident that no tunneling occures).</t>
+  </si>
+  <si>
+    <t>Menu is interacted with using the mouse. (Source.cpp line…)</t>
+  </si>
+  <si>
+    <t>Menus were self implemented (not based off of an example or using an API), they are made up of buttons and images, and interacted with using the mouse.</t>
+  </si>
+  <si>
+    <t>Camera.cpp</t>
+  </si>
+  <si>
+    <t>Source.cpp main method for example. There is no freeGLUT code used in this project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The camera class uses SLERP to calculate the orientation of the camera (aka the rotation). This is possible because the way the camera is modeled can be thought of as a point inside of a circle and rotating to face different points of the outside of the circle. </t>
+  </si>
+  <si>
+    <t>Used OpenGL texturing to texture some objects. Menus are not made of up simple colored objects, the images shown are made possible by texturing (with a texture shader, UVs, glGenTextures, etc), something we have not discussed in class.</t>
+  </si>
+  <si>
+    <t>Uses actual gravity interactions between bodies to produce rotation, movement, and orbits. It is awesome to explore what interactions occur and how they change based on position and other variables.</t>
+  </si>
+  <si>
+    <t>Thomas Bentley</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1254,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,13 +1860,13 @@
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
       <c r="E2" s="42" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F2" s="43"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44">
         <f>((F70/E70)*100)</f>
-        <v>96.428571428571431</v>
+        <v>139.28571428571428</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -1846,7 +1876,7 @@
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
       <c r="E3" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="43"/>
       <c r="G3" s="43"/>
@@ -1887,7 +1917,7 @@
       <c r="H5" s="48"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>62</v>
       </c>
@@ -1897,8 +1927,12 @@
       <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="6">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1914,7 +1948,7 @@
       </c>
       <c r="F7" s="9">
         <f>SUM(F6:F6)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
@@ -1945,7 +1979,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H9" s="13"/>
     </row>
@@ -1963,7 +1997,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H10" s="13"/>
     </row>
@@ -1981,7 +2015,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="13"/>
     </row>
@@ -1999,7 +2033,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -2047,7 +2081,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H15" s="13"/>
     </row>
@@ -2064,7 +2098,9 @@
       <c r="F16" s="12">
         <v>10</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,8 +2113,12 @@
       <c r="E17" s="12">
         <v>40</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="12">
+        <v>40</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2094,7 +2134,7 @@
       </c>
       <c r="F18" s="9">
         <f>SUM(F15:F17)</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
@@ -2124,10 +2164,12 @@
       <c r="F20" s="12">
         <v>5</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>16</v>
       </c>
@@ -2140,7 +2182,9 @@
       <c r="F21" s="12">
         <v>5</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2586,9 @@
       <c r="F52" s="12">
         <v>5</v>
       </c>
-      <c r="G52" s="13"/>
+      <c r="G52" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2559,7 +2605,7 @@
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
     </row>
-    <row r="54" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49" t="s">
         <v>74</v>
       </c>
@@ -2572,7 +2618,9 @@
       <c r="F54" s="12">
         <v>20</v>
       </c>
-      <c r="G54" s="13"/>
+      <c r="G54" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2585,8 +2633,12 @@
       <c r="E55" s="12">
         <v>10</v>
       </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="13"/>
+      <c r="F55" s="12">
+        <v>10</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="H55" s="13"/>
     </row>
     <row r="56" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,7 +2654,9 @@
       <c r="F56" s="12">
         <v>10</v>
       </c>
-      <c r="G56" s="13"/>
+      <c r="G56" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2674,7 +2728,9 @@
       <c r="F61" s="12">
         <v>10</v>
       </c>
-      <c r="G61" s="13"/>
+      <c r="G61" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2773,7 +2829,7 @@
       </c>
       <c r="F68" s="29"/>
       <c r="G68" s="22" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H68" s="22"/>
     </row>
@@ -2790,7 +2846,7 @@
       </c>
       <c r="F69" s="32">
         <f>SUM(F50:F68)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
@@ -2808,7 +2864,7 @@
       </c>
       <c r="F70" s="31">
         <f>MAX(0,SUM(F7,F13,F18,F23,F48,F69))</f>
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>

</xml_diff>